<commit_message>
read species and rxns, need to do propensities!
</commit_message>
<xml_diff>
--- a/model_definition.xlsx
+++ b/model_definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dex36\Documents\GitHub\ODBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB59330B-6273-42C9-80D2-6D27E4E3FF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E07AAA0-E95E-4B7E-BEC0-F270F1EB4937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5D4BE304-3618-4840-BED8-D27D0BA38927}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>5,10-CH-THF</t>
   </si>
   <si>
-    <t>h,10-CH2-THF</t>
-  </si>
-  <si>
     <t>THF</t>
   </si>
   <si>
@@ -248,6 +245,9 @@
   </si>
   <si>
     <t>5,10-CH2-THF; NADP+</t>
+  </si>
+  <si>
+    <t>5,10-CH2-THF</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +675,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
@@ -900,7 +900,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,6 +908,7 @@
     <col min="2" max="3" width="15.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="33.140625" style="2" customWidth="1"/>
     <col min="5" max="7" width="15.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -938,10 +939,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -952,24 +953,24 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -980,156 +981,156 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fmt, stoicheometry, mass action
</commit_message>
<xml_diff>
--- a/model_definition.xlsx
+++ b/model_definition.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\ODBM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dex36\Documents\GitHub\ODBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B550C-6EFA-4F3A-A0A3-7E83DF39E76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03ACE7A-8E32-4EC6-87AA-AAC3C0DAE601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="5130" windowWidth="20295" windowHeight="14085" xr2:uid="{5D4BE304-3618-4840-BED8-D27D0BA38927}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5D4BE304-3618-4840-BED8-D27D0BA38927}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
     <sheet name="Reaction" sheetId="3" r:id="rId2"/>
+    <sheet name="Mechanism Legend" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
   <si>
     <t>Label</t>
   </si>
@@ -254,6 +255,12 @@
   </si>
   <si>
     <t>DNA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>4 Serine</t>
   </si>
 </sst>
 </file>
@@ -627,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F5D3CC-A58A-4494-9B3C-2BFA219AC7F3}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="104" workbookViewId="0">
+    <sheetView zoomScale="104" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -1009,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26D5D16-1C04-425A-BBDB-1D98A70D3A08}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,11 +1061,20 @@
       <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1068,11 +1084,20 @@
       <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1082,11 +1107,20 @@
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1096,11 +1130,20 @@
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>69</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1110,11 +1153,20 @@
       <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1124,11 +1176,20 @@
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1138,11 +1199,20 @@
       <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1152,11 +1222,20 @@
       <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>58</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1166,11 +1245,20 @@
       <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1180,11 +1268,20 @@
       <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>62</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1194,11 +1291,20 @@
       <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>64</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1208,11 +1314,20 @@
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>66</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1222,11 +1337,20 @@
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1236,15 +1360,38 @@
       <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29F2506-6CCF-4DC4-9A74-8C4B207C7DA6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>